<commit_message>
More Tasks and Questions
</commit_message>
<xml_diff>
--- a/workspace/Tasks.xlsx
+++ b/workspace/Tasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Task</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Do I want any Sociology/Policy Classes for a CHS focus?</t>
+  </si>
+  <si>
+    <t>What pace should I be going through these articles?</t>
+  </si>
+  <si>
+    <t>How many articles should I cover in my survey presentation?</t>
   </si>
 </sst>
 </file>
@@ -125,7 +131,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -165,19 +171,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -205,8 +216,8 @@
   <tableColumns count="5">
     <tableColumn id="1" name="Task"/>
     <tableColumn id="2" name="Comments"/>
-    <tableColumn id="4" name="Due Date"/>
-    <tableColumn id="5" name="Done Date"/>
+    <tableColumn id="4" name="Due Date" dataDxfId="2"/>
+    <tableColumn id="5" name="Done Date" dataDxfId="1"/>
     <tableColumn id="3" name="Add Date" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -214,8 +225,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C6" totalsRowShown="0">
+  <autoFilter ref="A1:C6"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Question"/>
     <tableColumn id="2" name="Answer"/>
@@ -515,7 +526,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,13 +558,13 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>42508</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>42508</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>42507</v>
       </c>
     </row>
@@ -561,13 +572,13 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>42509</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>42509</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>42507</v>
       </c>
     </row>
@@ -575,13 +586,13 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>42508</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>42508</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>42507</v>
       </c>
     </row>
@@ -589,41 +600,41 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <v>42508</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>42508</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>42507</v>
       </c>
     </row>
     <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>42509</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>42509</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>42507</v>
       </c>
     </row>
     <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <v>42509</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>42509</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <v>42507</v>
       </c>
     </row>
@@ -631,11 +642,11 @@
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>42522</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
         <v>42518</v>
       </c>
     </row>
@@ -643,11 +654,11 @@
       <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>42522</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2">
         <v>42518</v>
       </c>
     </row>
@@ -655,53 +666,53 @@
       <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>42522</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2">
         <v>42518</v>
       </c>
     </row>
     <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>42522</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>42519</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>42518</v>
       </c>
     </row>
     <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>42522</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>42519</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>42518</v>
       </c>
     </row>
     <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>42522</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>42519</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>42518</v>
       </c>
     </row>
@@ -709,26 +720,26 @@
       <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>42577</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2">
         <v>42518</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>42583</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2">
         <v>42518</v>
       </c>
     </row>
@@ -736,10 +747,11 @@
       <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="1">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2">
         <v>42515</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="2">
         <v>42515</v>
       </c>
     </row>
@@ -747,10 +759,11 @@
       <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="1">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2">
         <v>42511</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="2">
         <v>42511</v>
       </c>
     </row>
@@ -758,11 +771,11 @@
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>42583</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2">
         <v>42518</v>
       </c>
     </row>
@@ -770,11 +783,11 @@
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>42583</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3">
+      <c r="D19" s="2"/>
+      <c r="E19" s="2">
         <v>42518</v>
       </c>
     </row>
@@ -782,37 +795,37 @@
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>42583</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3">
+      <c r="D20" s="2"/>
+      <c r="E20" s="2">
         <v>42518</v>
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="2">
         <v>42515</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="2">
         <v>42515</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="2">
         <v>42508</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>42583</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2">
         <v>42518</v>
       </c>
     </row>
@@ -820,10 +833,11 @@
       <c r="A23" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="2">
         <v>42583</v>
       </c>
-      <c r="E23" s="1">
+      <c r="D23" s="2"/>
+      <c r="E23" s="2">
         <v>42519</v>
       </c>
     </row>
@@ -848,10 +862,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,6 +898,16 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>